<commit_message>
Confusion on the excel solved
</commit_message>
<xml_diff>
--- a/Excels/DSU - DATA TRANSFROMATION v20250428.xlsx
+++ b/Excels/DSU - DATA TRANSFROMATION v20250428.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\WebApplication2\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14E8887-D513-4409-8699-06CC93F4AF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7843FAEE-7086-4AE7-9E27-37DA77DD5341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{053D180E-92F9-46FC-97EC-55500D712211}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{053D180E-92F9-46FC-97EC-55500D712211}"/>
   </bookViews>
   <sheets>
     <sheet name="HORIZONTAL" sheetId="1" r:id="rId1"/>
@@ -2360,7 +2360,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2699,17 +2699,16 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3050,7 +3049,7 @@
   <dimension ref="A1:LG9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CY1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="DC12" sqref="DC12"/>
+      <selection activeCell="CZ9" activeCellId="1" sqref="CY9 CZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7633,12 +7632,12 @@
       <c r="AQ9" s="115" t="s">
         <v>656</v>
       </c>
-      <c r="AR9" s="118" t="s">
+      <c r="AR9" s="122" t="s">
         <v>657</v>
       </c>
-      <c r="AS9" s="118"/>
-      <c r="AT9" s="118"/>
-      <c r="AU9" s="118"/>
+      <c r="AS9" s="122"/>
+      <c r="AT9" s="122"/>
+      <c r="AU9" s="122"/>
       <c r="AV9" s="115" t="s">
         <v>658</v>
       </c>
@@ -7672,9 +7671,9 @@
       <c r="BF9" s="115" t="s">
         <v>667</v>
       </c>
-      <c r="BG9" s="119"/>
-      <c r="BH9" s="119"/>
-      <c r="BI9" s="119"/>
+      <c r="BG9" s="118"/>
+      <c r="BH9" s="118"/>
+      <c r="BI9" s="118"/>
       <c r="BJ9" s="116" t="s">
         <v>669</v>
       </c>
@@ -7711,40 +7710,41 @@
       <c r="BU9" s="116" t="s">
         <v>631</v>
       </c>
-      <c r="BV9" s="119"/>
-      <c r="BW9" s="119"/>
+      <c r="BV9" s="118"/>
+      <c r="BW9" s="118"/>
       <c r="BX9" s="116"/>
-      <c r="BY9" s="119"/>
+      <c r="BY9" s="118"/>
       <c r="BZ9" s="116"/>
       <c r="CA9" s="116"/>
       <c r="CB9" s="116"/>
-      <c r="CC9" s="122" t="s">
+      <c r="CC9" s="123" t="s">
         <v>672</v>
       </c>
-      <c r="CD9" s="122"/>
-      <c r="CE9" s="122"/>
-      <c r="CF9" s="122"/>
-      <c r="CG9" s="122"/>
-      <c r="CH9" s="122"/>
-      <c r="CI9" s="122"/>
-      <c r="CJ9" s="123" t="s">
+      <c r="CD9" s="123"/>
+      <c r="CE9" s="123"/>
+      <c r="CF9" s="123"/>
+      <c r="CG9" s="123"/>
+      <c r="CH9" s="123"/>
+      <c r="CI9" s="123"/>
+      <c r="CJ9" s="121" t="s">
         <v>675</v>
       </c>
-      <c r="CK9" s="124"/>
-      <c r="CL9" s="124"/>
-      <c r="CM9" s="124"/>
-      <c r="CN9" s="124"/>
-      <c r="CO9" s="124"/>
-      <c r="CP9" s="124"/>
-      <c r="CQ9" s="124"/>
-      <c r="CR9" s="124"/>
-      <c r="CS9" s="124"/>
-      <c r="CT9" s="119"/>
-      <c r="CU9" s="119"/>
-      <c r="CV9" s="124"/>
-      <c r="CW9" s="124"/>
-      <c r="CX9" s="124"/>
-      <c r="CY9" s="124"/>
+      <c r="CK9" s="116"/>
+      <c r="CL9" s="116"/>
+      <c r="CM9" s="116"/>
+      <c r="CN9" s="116"/>
+      <c r="CO9" s="116"/>
+      <c r="CP9" s="116"/>
+      <c r="CQ9" s="116"/>
+      <c r="CR9" s="116"/>
+      <c r="CS9" s="116"/>
+      <c r="CT9" s="118"/>
+      <c r="CU9" s="118"/>
+      <c r="CV9" s="116"/>
+      <c r="CW9" s="116"/>
+      <c r="CX9" s="116"/>
+      <c r="CY9" s="116"/>
+      <c r="CZ9" s="116"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -8833,7 +8833,7 @@
       <c r="C81" t="s">
         <v>530</v>
       </c>
-      <c r="D81" s="120" t="s">
+      <c r="D81" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8847,7 +8847,7 @@
       <c r="C82" t="s">
         <v>531</v>
       </c>
-      <c r="D82" s="120" t="s">
+      <c r="D82" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8861,7 +8861,7 @@
       <c r="C83" t="s">
         <v>532</v>
       </c>
-      <c r="D83" s="120" t="s">
+      <c r="D83" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8875,7 +8875,7 @@
       <c r="C84" t="s">
         <v>533</v>
       </c>
-      <c r="D84" s="120" t="s">
+      <c r="D84" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8889,7 +8889,7 @@
       <c r="C85" t="s">
         <v>534</v>
       </c>
-      <c r="D85" s="120" t="s">
+      <c r="D85" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8903,7 +8903,7 @@
       <c r="C86" t="s">
         <v>535</v>
       </c>
-      <c r="D86" s="120" t="s">
+      <c r="D86" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8917,7 +8917,7 @@
       <c r="C87" t="s">
         <v>536</v>
       </c>
-      <c r="D87" s="120" t="s">
+      <c r="D87" s="119" t="s">
         <v>673</v>
       </c>
     </row>
@@ -8931,7 +8931,7 @@
       <c r="C88" t="s">
         <v>537</v>
       </c>
-      <c r="D88" s="121" t="s">
+      <c r="D88" s="120" t="s">
         <v>674</v>
       </c>
     </row>
@@ -8945,7 +8945,7 @@
       <c r="C89" t="s">
         <v>538</v>
       </c>
-      <c r="D89" s="121" t="s">
+      <c r="D89" s="120" t="s">
         <v>674</v>
       </c>
     </row>
@@ -10655,7 +10655,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>481</v>
       </c>
@@ -10808,21 +10808,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100555857D9FCE96B4E92A2FA640E16AE8E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75f8262ac504c833502fcdae4bc57a98">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c03aae23-ca47-43a3-8075-2f13d7789f4e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89e4d1ed8ada50da80f4f0e687ed4482" ns2:_="">
     <xsd:import namespace="c03aae23-ca47-43a3-8075-2f13d7789f4e"/>
@@ -10984,24 +10969,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E40FAE9C-4AD7-48EC-B3DA-F656BAD1FFEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43410EDF-71FA-4AF3-ACA6-94E67868039D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDF0E365-8122-426E-A98E-6C8BE0F976CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11017,4 +11000,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43410EDF-71FA-4AF3-ACA6-94E67868039D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E40FAE9C-4AD7-48EC-B3DA-F656BAD1FFEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>